<commit_message>
Screening & Template Update
</commit_message>
<xml_diff>
--- a/Business - Technology Services/KVYO.xlsx
+++ b/Business - Technology Services/KVYO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Business - Technology Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EDDFB3-5094-4810-8D86-E89549565F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001277CF-EDCA-4F27-83AE-4B6B5DA3748B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,30 +21,16 @@
     <sheet name="DoR" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Model!$B$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Model!$B$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Model!$J$16:$P$16</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Model!$J$16:$S$16</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Model!$J$17:$P$17</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Model!$J$17:$S$17</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Model!$J$2:$P$2</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Model!$J$2:$S$2</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Model!$B$3</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Model!$B$4</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Model!$J$2:$P$2</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Model!$J$2:$S$2</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Model!$J$2:$P$2</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Model!$J$3:$P$3</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Model!$J$3:$S$3</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Model!$J$4:$P$4</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Model!$J$4:$S$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Model!$J$2:$S$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Model!$J$3:$P$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Model!$J$3:$S$3</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Model!$J$4:$P$4</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Model!$J$4:$S$4</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Model!$B$16</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Model!$B$17</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Model!$B$16</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Model!$B$20</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Model!$J$16:$S$16</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Model!$J$20:$S$20</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Model!$J$2:$S$2</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Model!$B$3</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Model!$B$4</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Model!$J$2:$S$2</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Model!$J$3:$S$3</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Model!$J$4:$S$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -332,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="195">
   <si>
     <t>Price</t>
   </si>
@@ -908,6 +894,15 @@
   </si>
   <si>
     <t>Q424</t>
+  </si>
+  <si>
+    <t>SBC</t>
+  </si>
+  <si>
+    <t>Non-GAAP EPS</t>
+  </si>
+  <si>
+    <t>Non-GAAP Net Income</t>
   </si>
 </sst>
 </file>
@@ -1644,7 +1639,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1792,6 +1787,13 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="11" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="11" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1849,19 +1851,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1995,6 +1994,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4EEB-4735-AE8C-6B077AF8971C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2009,6 +2013,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4EEB-4735-AE8C-6B077AF8971C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2207,7 +2216,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$B$20</c:f>
+              <c:f>Model!$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2284,7 +2293,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Model!$J$20:$S$20</c:f>
+              <c:f>Model!$J$23:$S$23</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2851,7 +2860,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$B$20</c:f>
+              <c:f>Model!$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2938,7 +2947,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Model!$C$20:$G$20</c:f>
+              <c:f>Model!$C$23:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3328,6 +3337,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4AF1-4274-A25D-A2DF8B4EAB1F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -3342,6 +3356,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4AF1-4274-A25D-A2DF8B4EAB1F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -3540,7 +3559,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$B$18</c:f>
+              <c:f>Model!$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3617,7 +3636,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Model!$J$18:$S$18</c:f>
+              <c:f>Model!$J$21:$S$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4124,7 +4143,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$B$24</c:f>
+              <c:f>Model!$B$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4199,7 +4218,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Model!$C$24:$F$24</c:f>
+              <c:f>Model!$C$27:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4569,7 +4588,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$B$21</c:f>
+              <c:f>Model!$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4700,7 +4719,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Model!$J$21:$S$21</c:f>
+              <c:f>Model!$J$24:$S$24</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4743,7 +4762,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$B$22</c:f>
+              <c:f>Model!$B$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4874,7 +4893,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Model!$J$22:$S$22</c:f>
+              <c:f>Model!$J$25:$S$25</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4917,7 +4936,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Model!$B$23</c:f>
+              <c:f>Model!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5048,7 +5067,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Model!$J$23:$S$23</c:f>
+              <c:f>Model!$J$26:$S$26</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6127,18 +6146,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.15</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.13</cx:f>
+        <cx:f dir="row">_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.15</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.11</cx:f>
+        <cx:f dir="row">_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6182,7 +6201,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{006F4749-938E-4621-8334-C74E7B83CC40}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>EPS exp.</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6202,7 +6221,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C8A70830-D21B-405F-8F13-72F0AC678416}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>EPS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6233,18 +6252,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.3</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.7</cx:f>
+        <cx:f dir="row">_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.3</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.5</cx:f>
+        <cx:f dir="row">_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6288,7 +6307,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{006F4749-938E-4621-8334-C74E7B83CC40}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Rev. Exp.</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6308,7 +6327,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C8A70830-D21B-405F-8F13-72F0AC678416}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>Revenue</cx:v>
             </cx:txData>
           </cx:tx>
@@ -12240,7 +12259,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="15">
-        <f>Model!Q28</f>
+        <f>Model!Q31</f>
         <v>793.55499999999995</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -12354,7 +12373,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="36">
-        <f>C6/Model!F17</f>
+        <f>C6/Model!F20</f>
         <v>65.916666666666671</v>
       </c>
       <c r="E14" s="22"/>
@@ -12372,7 +12391,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="36">
-        <f>C6/Model!G17</f>
+        <f>C6/Model!G20</f>
         <v>54.551724137931039</v>
       </c>
     </row>
@@ -12389,15 +12408,15 @@
         <v>39</v>
       </c>
       <c r="C17" s="6">
-        <f>Model!G17/Model!F17-1</f>
+        <f>Model!G20/Model!F20-1</f>
         <v>0.20833333333333326</v>
       </c>
       <c r="E17" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="123"/>
-      <c r="M17" s="124"/>
-      <c r="N17" s="125"/>
+      <c r="L17" s="126"/>
+      <c r="M17" s="127"/>
+      <c r="N17" s="128"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
@@ -12407,9 +12426,9 @@
         <f>C14/(C16*100)</f>
         <v>0.65916666666666668</v>
       </c>
-      <c r="L18" s="126"/>
-      <c r="M18" s="127"/>
-      <c r="N18" s="128"/>
+      <c r="L18" s="129"/>
+      <c r="M18" s="130"/>
+      <c r="N18" s="131"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
@@ -12419,9 +12438,9 @@
         <f>C15/(C17*100)</f>
         <v>2.6184827586206909</v>
       </c>
-      <c r="L19" s="126"/>
-      <c r="M19" s="127"/>
-      <c r="N19" s="128"/>
+      <c r="L19" s="129"/>
+      <c r="M19" s="130"/>
+      <c r="N19" s="131"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -12431,9 +12450,9 @@
         <f>Model!F4/Model!E3-1</f>
         <v>0.31127533487370695</v>
       </c>
-      <c r="L20" s="126"/>
-      <c r="M20" s="127"/>
-      <c r="N20" s="128"/>
+      <c r="L20" s="129"/>
+      <c r="M20" s="130"/>
+      <c r="N20" s="131"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
@@ -12443,9 +12462,9 @@
         <f>Model!G4/Model!F4-1</f>
         <v>0.25628140703517599</v>
       </c>
-      <c r="L21" s="126"/>
-      <c r="M21" s="127"/>
-      <c r="N21" s="128"/>
+      <c r="L21" s="129"/>
+      <c r="M21" s="130"/>
+      <c r="N21" s="131"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
@@ -12455,9 +12474,9 @@
         <f>Model!E9+Model!E10</f>
         <v>-331.09199999999998</v>
       </c>
-      <c r="L22" s="126"/>
-      <c r="M22" s="127"/>
-      <c r="N22" s="128"/>
+      <c r="L22" s="129"/>
+      <c r="M22" s="130"/>
+      <c r="N22" s="131"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
@@ -12467,33 +12486,33 @@
         <f>Model!E12</f>
         <v>-307.04099999999994</v>
       </c>
-      <c r="L23" s="126"/>
-      <c r="M23" s="127"/>
-      <c r="N23" s="128"/>
+      <c r="L23" s="129"/>
+      <c r="M23" s="130"/>
+      <c r="N23" s="131"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="7">
-        <f>Model!Q18</f>
+        <f>Model!Q21</f>
         <v>0.77377111150112732</v>
       </c>
-      <c r="L24" s="126"/>
-      <c r="M24" s="127"/>
-      <c r="N24" s="128"/>
+      <c r="L24" s="129"/>
+      <c r="M24" s="130"/>
+      <c r="N24" s="131"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="7">
-        <f>Model!Q19</f>
+        <f>Model!Q22</f>
         <v>-2.2239922956802823E-2</v>
       </c>
-      <c r="L25" s="126"/>
-      <c r="M25" s="127"/>
-      <c r="N25" s="128"/>
+      <c r="L25" s="129"/>
+      <c r="M25" s="130"/>
+      <c r="N25" s="131"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
@@ -12503,9 +12522,9 @@
         <f>C12/C23</f>
         <v>-24.753444298839572</v>
       </c>
-      <c r="L26" s="126"/>
-      <c r="M26" s="127"/>
-      <c r="N26" s="128"/>
+      <c r="L26" s="129"/>
+      <c r="M26" s="130"/>
+      <c r="N26" s="131"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
@@ -12517,9 +12536,9 @@
       <c r="E27" t="s">
         <v>69</v>
       </c>
-      <c r="L27" s="126"/>
-      <c r="M27" s="127"/>
-      <c r="N27" s="128"/>
+      <c r="L27" s="129"/>
+      <c r="M27" s="130"/>
+      <c r="N27" s="131"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -12531,16 +12550,16 @@
       <c r="E28" t="s">
         <v>167</v>
       </c>
-      <c r="L28" s="129"/>
-      <c r="M28" s="130"/>
-      <c r="N28" s="131"/>
+      <c r="L28" s="132"/>
+      <c r="M28" s="133"/>
+      <c r="N28" s="134"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C29" s="36">
-        <f>Model!Q33/Model!Q45</f>
+        <f>Model!Q36/Model!Q48</f>
         <v>6.628243410605335</v>
       </c>
     </row>
@@ -12549,7 +12568,7 @@
         <v>81</v>
       </c>
       <c r="C30" s="36">
-        <f>(Model!Q28+Model!Q29+Model!Q30)/Model!Q45</f>
+        <f>(Model!Q31+Model!Q32+Model!Q33)/Model!Q48</f>
         <v>6.2545721167361883</v>
       </c>
     </row>
@@ -12564,7 +12583,7 @@
         <v>83</v>
       </c>
       <c r="C32" s="36">
-        <f>(Model!Q27-Model!Q35)/Main!C7</f>
+        <f>(Model!Q30-Model!Q38)/Main!C7</f>
         <v>2.8718563453341859</v>
       </c>
     </row>
@@ -12579,7 +12598,7 @@
         <v>85</v>
       </c>
       <c r="C34" s="38">
-        <f>Model!E14/Model!E40</f>
+        <f>Model!E14/Model!E43</f>
         <v>-0.28302924567283411</v>
       </c>
     </row>
@@ -12588,7 +12607,7 @@
         <v>86</v>
       </c>
       <c r="C35" s="38">
-        <f>Model!E14/Model!E49</f>
+        <f>Model!E14/Model!E52</f>
         <v>-0.3369487864255441</v>
       </c>
     </row>
@@ -12609,13 +12628,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7345E9-1C5F-45F5-BD7C-66FA029FFFF4}">
-  <dimension ref="A1:S70"/>
+  <dimension ref="A1:S73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X20" sqref="X20"/>
+      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12623,7 +12642,6 @@
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="13"/>
-    <col min="15" max="15" width="11.42578125" style="142"/>
     <col min="17" max="17" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
@@ -12663,7 +12681,7 @@
       <c r="N2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="142" t="s">
+      <c r="O2" t="s">
         <v>35</v>
       </c>
       <c r="P2" t="s">
@@ -12713,19 +12731,19 @@
       <c r="N3" s="10">
         <v>175.80699999999999</v>
       </c>
-      <c r="O3" s="143">
+      <c r="O3" s="10">
         <v>201.61799999999999</v>
       </c>
-      <c r="P3" s="143">
+      <c r="P3" s="10">
         <v>209.99299999999999</v>
       </c>
       <c r="Q3" s="15">
         <v>222.21299999999999</v>
       </c>
-      <c r="R3" s="143">
+      <c r="R3" s="10">
         <v>226.04</v>
       </c>
-      <c r="S3" s="143">
+      <c r="S3" s="10">
         <v>256.91000000000003</v>
       </c>
     </row>
@@ -12747,17 +12765,17 @@
       <c r="L4" s="40"/>
       <c r="M4" s="40"/>
       <c r="N4" s="40"/>
-      <c r="O4" s="143"/>
-      <c r="P4" s="143">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10">
         <v>202.21</v>
       </c>
       <c r="Q4" s="15">
         <v>209.99</v>
       </c>
-      <c r="R4" s="143">
+      <c r="R4" s="10">
         <v>226.04</v>
       </c>
-      <c r="S4" s="143">
+      <c r="S4" s="10">
         <v>256.91000000000003</v>
       </c>
     </row>
@@ -12791,17 +12809,17 @@
       <c r="N5" s="10">
         <v>58.825000000000003</v>
       </c>
-      <c r="O5" s="143">
+      <c r="O5" s="10">
         <v>45.012999999999998</v>
       </c>
-      <c r="P5" s="143">
+      <c r="P5" s="10">
         <v>44.938000000000002</v>
       </c>
       <c r="Q5" s="15">
         <v>50.271000000000001</v>
       </c>
-      <c r="R5" s="143"/>
-      <c r="S5" s="143"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -12833,17 +12851,17 @@
       <c r="N6" s="10">
         <v>167.87700000000001</v>
       </c>
-      <c r="O6" s="143">
+      <c r="O6" s="10">
         <v>102.524</v>
       </c>
-      <c r="P6" s="143">
+      <c r="P6" s="10">
         <v>91.858000000000004</v>
       </c>
       <c r="Q6" s="15">
         <v>94.501000000000005</v>
       </c>
-      <c r="R6" s="143"/>
-      <c r="S6" s="143"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -12875,17 +12893,17 @@
       <c r="N7" s="10">
         <v>141.45500000000001</v>
       </c>
-      <c r="O7" s="143">
+      <c r="O7" s="10">
         <v>52.634999999999998</v>
       </c>
-      <c r="P7" s="143">
+      <c r="P7" s="10">
         <v>56.097000000000001</v>
       </c>
       <c r="Q7" s="15">
         <v>55.734999999999999</v>
       </c>
-      <c r="R7" s="143"/>
-      <c r="S7" s="143"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -12917,17 +12935,17 @@
       <c r="N8" s="10">
         <v>109.85299999999999</v>
       </c>
-      <c r="O8" s="143">
+      <c r="O8" s="10">
         <v>37.776000000000003</v>
       </c>
-      <c r="P8" s="143">
+      <c r="P8" s="10">
         <v>39.192</v>
       </c>
       <c r="Q8" s="15">
         <v>35.759</v>
       </c>
-      <c r="R8" s="143"/>
-      <c r="S8" s="143"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -12975,11 +12993,11 @@
         <f t="shared" si="0"/>
         <v>-302.20300000000009</v>
       </c>
-      <c r="O9" s="144">
+      <c r="O9" s="11">
         <f t="shared" si="0"/>
         <v>-36.330000000000013</v>
       </c>
-      <c r="P9" s="144">
+      <c r="P9" s="11">
         <f t="shared" si="0"/>
         <v>-22.092000000000013</v>
       </c>
@@ -12987,11 +13005,11 @@
         <f t="shared" si="0"/>
         <v>-14.053000000000026</v>
       </c>
-      <c r="R9" s="144">
+      <c r="R9" s="11">
         <f t="shared" ref="R9:S9" si="1">R3-SUM(R5:R8)</f>
         <v>226.04</v>
       </c>
-      <c r="S9" s="144">
+      <c r="S9" s="11">
         <f t="shared" si="1"/>
         <v>256.91000000000003</v>
       </c>
@@ -13026,17 +13044,17 @@
       <c r="N10" s="10">
         <v>0.26500000000000001</v>
       </c>
-      <c r="O10" s="143">
+      <c r="O10" s="10">
         <v>-0.126</v>
       </c>
-      <c r="P10" s="143">
+      <c r="P10" s="10">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="Q10" s="15">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="R10" s="143"/>
-      <c r="S10" s="143"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -13068,17 +13086,17 @@
       <c r="N11" s="10">
         <v>6.1829999999999998</v>
       </c>
-      <c r="O11" s="143">
+      <c r="O11" s="10">
         <v>9.5670000000000002</v>
       </c>
-      <c r="P11" s="143">
+      <c r="P11" s="10">
         <v>9.5459999999999994</v>
       </c>
       <c r="Q11" s="15">
         <v>9.9789999999999992</v>
       </c>
-      <c r="R11" s="143"/>
-      <c r="S11" s="143"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
     </row>
     <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -13124,11 +13142,11 @@
         <f t="shared" si="2"/>
         <v>-295.75500000000011</v>
       </c>
-      <c r="O12" s="144">
+      <c r="O12" s="11">
         <f t="shared" si="2"/>
         <v>-26.88900000000001</v>
       </c>
-      <c r="P12" s="144">
+      <c r="P12" s="11">
         <f t="shared" si="2"/>
         <v>-12.478000000000014</v>
       </c>
@@ -13136,11 +13154,11 @@
         <f t="shared" si="2"/>
         <v>-4.0810000000000262</v>
       </c>
-      <c r="R12" s="144">
+      <c r="R12" s="11">
         <f t="shared" ref="R12:S12" si="3">R9+SUM(R10:R11)</f>
         <v>226.04</v>
       </c>
-      <c r="S12" s="144">
+      <c r="S12" s="11">
         <f t="shared" si="3"/>
         <v>256.91000000000003</v>
       </c>
@@ -13175,17 +13193,17 @@
       <c r="N13" s="10">
         <v>0.81899999999999995</v>
       </c>
-      <c r="O13" s="143">
+      <c r="O13" s="10">
         <v>-0.59399999999999997</v>
       </c>
-      <c r="P13" s="143">
+      <c r="P13" s="10">
         <v>0.40400000000000003</v>
       </c>
       <c r="Q13" s="15">
         <v>0.86099999999999999</v>
       </c>
-      <c r="R13" s="143"/>
-      <c r="S13" s="143"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
     </row>
     <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -13225,11 +13243,11 @@
         <f t="shared" si="4"/>
         <v>-296.57400000000013</v>
       </c>
-      <c r="O14" s="144">
+      <c r="O14" s="11">
         <f t="shared" si="4"/>
         <v>-26.295000000000009</v>
       </c>
-      <c r="P14" s="144">
+      <c r="P14" s="11">
         <f t="shared" si="4"/>
         <v>-12.882000000000014</v>
       </c>
@@ -13237,11 +13255,11 @@
         <f t="shared" si="4"/>
         <v>-4.9420000000000259</v>
       </c>
-      <c r="R14" s="144">
+      <c r="R14" s="11">
         <f>R16*R15</f>
         <v>29.182253539999998</v>
       </c>
-      <c r="S14" s="144">
+      <c r="S14" s="11">
         <f>S16*S15</f>
         <v>26.529321400000001</v>
       </c>
@@ -13276,19 +13294,19 @@
       <c r="N15" s="10">
         <v>240.125168</v>
       </c>
-      <c r="O15" s="143">
+      <c r="O15" s="10">
         <v>258.89918899999998</v>
       </c>
-      <c r="P15" s="143">
+      <c r="P15" s="10">
         <v>261.33241099999998</v>
       </c>
       <c r="Q15" s="15">
         <v>265.29321399999998</v>
       </c>
-      <c r="R15" s="143">
+      <c r="R15" s="10">
         <v>265.29321399999998</v>
       </c>
-      <c r="S15" s="143">
+      <c r="S15" s="10">
         <v>265.29321399999998</v>
       </c>
     </row>
@@ -13315,1184 +13333,1143 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="J16" s="2">
-        <f>J14/J15</f>
+        <f t="shared" ref="J16:Q16" si="5">J14/J15</f>
         <v>-0.10291273740040068</v>
       </c>
       <c r="K16" s="2">
-        <f>K14/K15</f>
+        <f t="shared" si="5"/>
         <v>-3.218877139518345E-3</v>
       </c>
       <c r="L16" s="2">
-        <f>L14/L15</f>
+        <f t="shared" si="5"/>
         <v>1.8165759369506387E-2</v>
       </c>
       <c r="M16" s="2">
-        <f>M14/M15</f>
+        <f t="shared" si="5"/>
         <v>4.6016269437324876E-2</v>
       </c>
       <c r="N16" s="2">
-        <f>N14/N15</f>
+        <f t="shared" si="5"/>
         <v>-1.2350808641599789</v>
       </c>
-      <c r="O16" s="145">
-        <f>O14/O15</f>
+      <c r="O16" s="123">
+        <f t="shared" si="5"/>
         <v>-0.101564628694144</v>
       </c>
-      <c r="P16" s="145">
-        <f>P14/P15</f>
+      <c r="P16" s="123">
+        <f t="shared" si="5"/>
         <v>-4.9293541320445E-2</v>
       </c>
       <c r="Q16" s="54">
-        <f>Q14/Q15</f>
+        <f t="shared" si="5"/>
         <v>-1.8628444827088666E-2</v>
       </c>
-      <c r="R16" s="150">
+      <c r="R16" s="125">
         <v>0.11</v>
       </c>
-      <c r="S16" s="150">
+      <c r="S16" s="125">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+    <row r="17" spans="2:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="147" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" s="148"/>
+      <c r="D17" s="148"/>
+      <c r="E17" s="149"/>
+      <c r="F17" s="150"/>
+      <c r="G17" s="151"/>
+      <c r="J17" s="148"/>
+      <c r="K17" s="148"/>
+      <c r="L17" s="148"/>
+      <c r="M17" s="148">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="N17" s="148"/>
+      <c r="O17" s="152"/>
+      <c r="P17" s="152">
+        <v>35.753999999999998</v>
+      </c>
+      <c r="Q17" s="153">
+        <v>35.316000000000003</v>
+      </c>
+      <c r="R17" s="125"/>
+      <c r="S17" s="125"/>
+    </row>
+    <row r="18" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="154">
+        <f>M14+M17</f>
+        <v>11.406000000000011</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="145"/>
+      <c r="P18" s="154">
+        <f>P14+P17</f>
+        <v>22.871999999999986</v>
+      </c>
+      <c r="Q18" s="146">
+        <f>Q14+Q17</f>
+        <v>30.373999999999977</v>
+      </c>
+      <c r="R18" s="125"/>
+      <c r="S18" s="125"/>
+    </row>
+    <row r="19" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="154">
+        <f>M18/M15</f>
+        <v>4.8209935629845463E-2</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="145"/>
+      <c r="P19" s="154">
+        <f>P18/P15</f>
+        <v>8.7520717053347005E-2</v>
+      </c>
+      <c r="Q19" s="146">
+        <f>Q18/Q15</f>
+        <v>0.11449218599311771</v>
+      </c>
+      <c r="R19" s="125"/>
+      <c r="S19" s="125"/>
+    </row>
+    <row r="20" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="44">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="44">
         <v>0.48</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G20" s="45">
         <v>0.57999999999999996</v>
       </c>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="146"/>
-      <c r="P17" s="146">
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="124"/>
+      <c r="P20" s="124">
         <v>0.11</v>
       </c>
-      <c r="Q17" s="49">
+      <c r="Q20" s="49">
         <v>0.1</v>
       </c>
-      <c r="R17" s="146">
+      <c r="R20" s="124">
         <v>0.11</v>
       </c>
-      <c r="S17" s="146">
+      <c r="S20" s="124">
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="21" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C21" s="3">
         <f>1-C5/C3</f>
         <v>0.70858794384805945</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D21" s="3">
         <f>1-D5/D3</f>
         <v>0.72918975860289204</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E21" s="6">
         <f>1-E5/E3</f>
         <v>0.7451822735743785</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="J18" s="3">
-        <f t="shared" ref="J18:P18" si="5">1-J5/J3</f>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="J21" s="3">
+        <f t="shared" ref="J21:P21" si="6">1-J5/J3</f>
         <v>0.72627718850698175</v>
       </c>
-      <c r="K18" s="3">
-        <f t="shared" si="5"/>
+      <c r="K21" s="3">
+        <f t="shared" si="6"/>
         <v>0.74296140737425553</v>
       </c>
-      <c r="L18" s="3">
-        <f t="shared" si="5"/>
+      <c r="L21" s="3">
+        <f t="shared" si="6"/>
         <v>0.76568346061196246</v>
       </c>
-      <c r="M18" s="3">
-        <f t="shared" si="5"/>
+      <c r="M21" s="3">
+        <f t="shared" si="6"/>
         <v>0.7723014108125843</v>
       </c>
-      <c r="N18" s="3">
-        <f t="shared" si="5"/>
+      <c r="N21" s="3">
+        <f t="shared" si="6"/>
         <v>0.66540012627483547</v>
       </c>
-      <c r="O18" s="39">
-        <f t="shared" si="5"/>
+      <c r="O21" s="39">
+        <f t="shared" si="6"/>
         <v>0.77674116398337456</v>
       </c>
-      <c r="P18" s="39">
-        <f t="shared" si="5"/>
+      <c r="P21" s="39">
+        <f t="shared" si="6"/>
         <v>0.78600239055587562</v>
       </c>
-      <c r="Q18" s="6">
-        <f t="shared" ref="Q18" si="6">1-Q5/Q3</f>
+      <c r="Q21" s="6">
+        <f t="shared" ref="Q21" si="7">1-Q5/Q3</f>
         <v>0.77377111150112732</v>
       </c>
-      <c r="R18" s="39"/>
-      <c r="S18" s="39"/>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C22" s="4">
         <f>C14/C3</f>
         <v>-0.27313859069639418</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D22" s="4">
         <f>D14/D3</f>
         <v>-0.10405755286114401</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E22" s="7">
         <f>E14/E3</f>
         <v>-0.44153193171742106</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F22" s="47">
         <f>F14/F4</f>
         <v>0</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G22" s="47">
         <f>G14/G4</f>
         <v>0</v>
       </c>
-      <c r="J19" s="4">
-        <f t="shared" ref="J19:P19" si="7">J14/J3</f>
+      <c r="J22" s="4">
+        <f t="shared" ref="J22:P22" si="8">J14/J3</f>
         <v>-0.20033062567132126</v>
       </c>
-      <c r="K19" s="4">
-        <f t="shared" si="7"/>
+      <c r="K22" s="4">
+        <f t="shared" si="8"/>
         <v>-5.198471442834013E-3</v>
       </c>
-      <c r="L19" s="4">
-        <f t="shared" si="7"/>
+      <c r="L22" s="4">
+        <f t="shared" si="8"/>
         <v>2.7407616216493354E-2</v>
       </c>
-      <c r="M19" s="4">
-        <f t="shared" si="7"/>
+      <c r="M22" s="4">
+        <f t="shared" si="8"/>
         <v>6.6147788997849205E-2</v>
       </c>
-      <c r="N19" s="4">
-        <f t="shared" si="7"/>
+      <c r="N22" s="4">
+        <f t="shared" si="8"/>
         <v>-1.686929416917416</v>
       </c>
-      <c r="O19" s="147">
-        <f t="shared" si="7"/>
+      <c r="O22" s="4">
+        <f t="shared" si="8"/>
         <v>-0.13041990298485259</v>
       </c>
-      <c r="P19" s="147">
-        <f t="shared" si="7"/>
+      <c r="P22" s="4">
+        <f t="shared" si="8"/>
         <v>-6.1344901972922972E-2</v>
       </c>
-      <c r="Q19" s="7">
-        <f t="shared" ref="Q19" si="8">Q14/Q3</f>
+      <c r="Q22" s="7">
+        <f t="shared" ref="Q22" si="9">Q14/Q3</f>
         <v>-2.2239922956802823E-2</v>
       </c>
-      <c r="R19" s="147"/>
-      <c r="S19" s="147"/>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="39">
+      <c r="C23" s="3"/>
+      <c r="D23" s="39">
         <f>D3/C3-1</f>
         <v>0.6265758326451969</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E23" s="6">
         <f>E3/D3-1</f>
         <v>0.47668313773934545</v>
       </c>
-      <c r="F20" s="48">
+      <c r="F23" s="48">
         <f>F4/E3-1</f>
         <v>0.31127533487370695</v>
       </c>
-      <c r="G20" s="48">
+      <c r="G23" s="48">
         <f>G4/F4-1</f>
         <v>0.25628140703517599</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4">
-        <f t="shared" ref="N20:O20" si="9">N3/J3-1</f>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4">
+        <f t="shared" ref="N23:O23" si="10">N3/J3-1</f>
         <v>0.47528698979591821</v>
       </c>
-      <c r="O20" s="147">
-        <f t="shared" si="9"/>
+      <c r="O23" s="4">
+        <f t="shared" si="10"/>
         <v>0.38821909319378922</v>
       </c>
-      <c r="P20" s="147">
+      <c r="P23" s="4">
         <f>P3/L3-1</f>
         <v>0.34535005894111026</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q23" s="7">
         <f>Q3/M3-1</f>
         <v>0.35013306113521181</v>
       </c>
-      <c r="R20" s="147">
+      <c r="R23" s="4">
         <f>R3/N3-1</f>
         <v>0.28572809956372613</v>
       </c>
-      <c r="S20" s="147">
+      <c r="S23" s="4">
         <f>S3/O3-1</f>
         <v>0.27424138717773228</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C24" s="4">
         <f>C6/C3</f>
         <v>0.53792320396366644</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D24" s="4">
         <f>D6/D3</f>
         <v>0.45235093538206406</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E24" s="7">
         <f>E6/E3</f>
         <v>0.56491844279966019</v>
       </c>
-      <c r="F21" s="120"/>
-      <c r="G21" s="120"/>
-      <c r="J21" s="4">
-        <f t="shared" ref="J21:P21" si="10">J6/J3</f>
+      <c r="F24" s="120"/>
+      <c r="G24" s="120"/>
+      <c r="J24" s="4">
+        <f t="shared" ref="J24:P24" si="11">J6/J3</f>
         <v>0.51592709452201935</v>
       </c>
-      <c r="K21" s="4">
-        <f t="shared" si="10"/>
+      <c r="K24" s="4">
+        <f t="shared" si="11"/>
         <v>0.41620132888077943</v>
       </c>
-      <c r="L21" s="4">
-        <f t="shared" si="10"/>
+      <c r="L24" s="4">
+        <f t="shared" si="11"/>
         <v>0.38832581620624262</v>
       </c>
-      <c r="M21" s="4">
-        <f t="shared" si="10"/>
+      <c r="M24" s="4">
+        <f t="shared" si="11"/>
         <v>0.38494768692355363</v>
       </c>
-      <c r="N21" s="4">
-        <f t="shared" si="10"/>
+      <c r="N24" s="4">
+        <f t="shared" si="11"/>
         <v>0.95489371868014372</v>
       </c>
-      <c r="O21" s="147">
-        <f t="shared" si="10"/>
+      <c r="O24" s="4">
+        <f t="shared" si="11"/>
         <v>0.50850618496364408</v>
       </c>
-      <c r="P21" s="147">
-        <f t="shared" si="10"/>
+      <c r="P24" s="4">
+        <f t="shared" si="11"/>
         <v>0.43743362874000563</v>
       </c>
-      <c r="Q21" s="7">
-        <f t="shared" ref="Q21" si="11">Q6/Q3</f>
+      <c r="Q24" s="7">
+        <f t="shared" ref="Q24" si="12">Q6/Q3</f>
         <v>0.42527214879417496</v>
       </c>
-      <c r="R21" s="147"/>
-      <c r="S21" s="147"/>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C25" s="4">
         <f>C7/C3</f>
         <v>0.225705339939444</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D25" s="4">
         <f>D7/D3</f>
         <v>0.2201532317429159</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E25" s="7">
         <f>E7/E3</f>
         <v>0.37555848096043687</v>
       </c>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="J22" s="4">
-        <f t="shared" ref="J22:O22" si="12">J7/J3</f>
+      <c r="F25" s="120"/>
+      <c r="G25" s="120"/>
+      <c r="J25" s="4">
+        <f t="shared" ref="J25:O25" si="13">J7/J3</f>
         <v>0.25250067132116005</v>
       </c>
-      <c r="K22" s="4">
-        <f t="shared" si="12"/>
+      <c r="K25" s="4">
+        <f t="shared" si="13"/>
         <v>0.19769339346576237</v>
       </c>
-      <c r="L22" s="4">
-        <f t="shared" si="12"/>
+      <c r="L25" s="4">
+        <f t="shared" si="13"/>
         <v>0.22443749679667879</v>
       </c>
-      <c r="M22" s="4">
-        <f t="shared" si="12"/>
+      <c r="M25" s="4">
+        <f t="shared" si="13"/>
         <v>0.20083725225717861</v>
       </c>
-      <c r="N22" s="4">
-        <f t="shared" si="12"/>
+      <c r="N25" s="4">
+        <f t="shared" si="13"/>
         <v>0.80460391224467753</v>
       </c>
-      <c r="O22" s="147">
-        <f t="shared" si="12"/>
+      <c r="O25" s="4">
+        <f t="shared" si="13"/>
         <v>0.26106300032735175</v>
       </c>
-      <c r="P22" s="147">
-        <f t="shared" ref="P22:Q22" si="13">P7/P3</f>
+      <c r="P25" s="4">
+        <f t="shared" ref="P25:Q25" si="14">P7/P3</f>
         <v>0.26713747601110516</v>
       </c>
-      <c r="Q22" s="7">
-        <f t="shared" si="13"/>
+      <c r="Q25" s="7">
+        <f t="shared" si="14"/>
         <v>0.25081790894322115</v>
       </c>
-      <c r="R22" s="147"/>
-      <c r="S22" s="147"/>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="4">
-        <f t="shared" ref="C23" si="14">C8/C3</f>
+      <c r="C26" s="4">
+        <f t="shared" ref="C26" si="15">C8/C3</f>
         <v>0.21757500688136527</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D26" s="4">
         <f>D8/D3</f>
         <v>0.17310279472361598</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E26" s="7">
         <f>E8/E3</f>
         <v>0.27830866395740433</v>
       </c>
-      <c r="F23" s="120"/>
-      <c r="G23" s="120"/>
-      <c r="J23" s="4">
-        <f t="shared" ref="J23:O23" si="15">J8/J3</f>
+      <c r="F26" s="120"/>
+      <c r="G26" s="120"/>
+      <c r="J26" s="4">
+        <f t="shared" ref="J26:O26" si="16">J8/J3</f>
         <v>0.17320085929108486</v>
       </c>
-      <c r="K23" s="4">
-        <f t="shared" si="15"/>
+      <c r="K26" s="4">
+        <f t="shared" si="16"/>
         <v>0.15713843081901743</v>
       </c>
-      <c r="L23" s="4">
-        <f t="shared" si="15"/>
+      <c r="L26" s="4">
+        <f t="shared" si="16"/>
         <v>0.14729511557582903</v>
       </c>
-      <c r="M23" s="4">
-        <f t="shared" si="15"/>
+      <c r="M26" s="4">
+        <f t="shared" si="16"/>
         <v>0.14379108794186624</v>
       </c>
-      <c r="N23" s="4">
-        <f t="shared" si="15"/>
+      <c r="N26" s="4">
+        <f t="shared" si="16"/>
         <v>0.62484997753218019</v>
       </c>
-      <c r="O23" s="147">
-        <f t="shared" si="15"/>
+      <c r="O26" s="4">
+        <f t="shared" si="16"/>
         <v>0.18736422343243164</v>
       </c>
-      <c r="P23" s="147">
-        <f t="shared" ref="P23:Q23" si="16">P8/P3</f>
+      <c r="P26" s="4">
+        <f t="shared" ref="P26:Q26" si="17">P8/P3</f>
         <v>0.18663479258832438</v>
       </c>
-      <c r="Q23" s="7">
-        <f t="shared" si="16"/>
+      <c r="Q26" s="7">
+        <f t="shared" si="17"/>
         <v>0.16092217827039823</v>
       </c>
-      <c r="R23" s="147"/>
-      <c r="S23" s="147"/>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="39">
+      <c r="C27" s="3"/>
+      <c r="D27" s="39">
         <f>D14/C14-1</f>
         <v>-0.38032373874157455</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E27" s="6">
         <f>E14/D14-1</f>
         <v>5.2657898481491117</v>
       </c>
-      <c r="F24" s="57">
-        <f>F17/E16-1</f>
+      <c r="F27" s="57">
+        <f>F20/E16-1</f>
         <v>-1.3782425975155159</v>
       </c>
-      <c r="G24" s="57">
-        <f>G17/F17-1</f>
+      <c r="G27" s="57">
+        <f>G20/F20-1</f>
         <v>0.20833333333333326</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4">
-        <f t="shared" ref="N24:S24" si="17">N14/J14-1</f>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4">
+        <f t="shared" ref="N27:S27" si="18">N14/J14-1</f>
         <v>11.422988313157122</v>
       </c>
-      <c r="O24" s="147">
-        <f t="shared" si="17"/>
+      <c r="O27" s="4">
+        <f t="shared" si="18"/>
         <v>33.827814569536535</v>
       </c>
-      <c r="P24" s="147">
-        <f t="shared" si="17"/>
+      <c r="P27" s="4">
+        <f t="shared" si="18"/>
         <v>-4.0112201963534293</v>
       </c>
-      <c r="Q24" s="7">
-        <f t="shared" si="17"/>
+      <c r="Q27" s="7">
+        <f t="shared" si="18"/>
         <v>-1.4539358868375145</v>
       </c>
-      <c r="R24" s="147">
-        <f t="shared" si="17"/>
+      <c r="R27" s="4">
+        <f t="shared" si="18"/>
         <v>-1.0983978822823308</v>
       </c>
-      <c r="S24" s="147">
-        <f t="shared" si="17"/>
+      <c r="S27" s="4">
+        <f t="shared" si="18"/>
         <v>-2.0089112530899405</v>
       </c>
     </row>
-    <row r="27" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+    <row r="30" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="11">
-        <f t="shared" ref="C27" si="18">C28+C29</f>
+      <c r="C30" s="11">
+        <f t="shared" ref="C30" si="19">C31+C32</f>
         <v>0</v>
       </c>
-      <c r="D27" s="11">
-        <f>D28+D29</f>
+      <c r="D30" s="11">
+        <f>D31+D32</f>
         <v>386.22899999999998</v>
       </c>
-      <c r="E27" s="14">
-        <f>E28+E29</f>
+      <c r="E30" s="14">
+        <f>E31+E32</f>
         <v>738.971</v>
       </c>
-      <c r="J27" s="11">
-        <f t="shared" ref="J27:N27" si="19">J28+J29</f>
+      <c r="J30" s="11">
+        <f t="shared" ref="J30:N30" si="20">J31+J32</f>
         <v>0</v>
       </c>
-      <c r="K27" s="11">
-        <f t="shared" si="19"/>
+      <c r="K30" s="11">
+        <f t="shared" si="20"/>
         <v>386.22899999999998</v>
       </c>
-      <c r="L27" s="11">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="11">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="11">
-        <f t="shared" si="19"/>
-        <v>723.80099999999993</v>
-      </c>
-      <c r="O27" s="144">
-        <f>O28+O29</f>
-        <v>738.971</v>
-      </c>
-      <c r="P27" s="11">
-        <f t="shared" ref="P27:S27" si="20">P28+P29</f>
-        <v>756.22</v>
-      </c>
-      <c r="Q27" s="14">
-        <f t="shared" si="20"/>
-        <v>793.95699999999999</v>
-      </c>
-      <c r="R27" s="11">
+      <c r="L30" s="11">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="S27" s="11">
+      <c r="M30" s="11">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10">
-        <v>385.82</v>
-      </c>
-      <c r="E28" s="15">
-        <v>738.56200000000001</v>
-      </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10">
-        <f>D28</f>
-        <v>385.82</v>
-      </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10">
-        <v>723.41499999999996</v>
-      </c>
-      <c r="O28" s="143">
-        <f>E28</f>
-        <v>738.56200000000001</v>
-      </c>
-      <c r="P28" s="10">
-        <v>755.827</v>
-      </c>
-      <c r="Q28" s="15">
-        <v>793.55499999999995</v>
-      </c>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="E29" s="15">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10">
-        <f>D29</f>
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="O29" s="143">
-        <f>E29</f>
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="P29" s="10">
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="Q29" s="15">
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10">
-        <v>10.723000000000001</v>
-      </c>
-      <c r="E30" s="15">
-        <v>23.076000000000001</v>
-      </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10">
-        <f>D30</f>
-        <v>10.723000000000001</v>
-      </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10">
-        <v>17.38</v>
-      </c>
-      <c r="O30" s="143">
-        <f>E30</f>
-        <v>23.076000000000001</v>
-      </c>
-      <c r="P30" s="10">
-        <v>23.241</v>
-      </c>
-      <c r="Q30" s="15">
-        <v>29.225999999999999</v>
-      </c>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
+      <c r="N30" s="11">
+        <f t="shared" si="20"/>
+        <v>723.80099999999993</v>
+      </c>
+      <c r="O30" s="11">
+        <f>O31+O32</f>
+        <v>738.971</v>
+      </c>
+      <c r="P30" s="11">
+        <f t="shared" ref="P30:S30" si="21">P31+P32</f>
+        <v>756.22</v>
+      </c>
+      <c r="Q30" s="14">
+        <f t="shared" si="21"/>
+        <v>793.95699999999999</v>
+      </c>
+      <c r="R30" s="11">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S30" s="11">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>159</v>
+        <v>18</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10">
-        <v>11.215</v>
+        <v>385.82</v>
       </c>
       <c r="E31" s="15">
-        <v>15.198</v>
+        <v>738.56200000000001</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10">
         <f>D31</f>
-        <v>11.215</v>
+        <v>385.82</v>
       </c>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10">
-        <v>14.161</v>
-      </c>
-      <c r="O31" s="143">
+        <v>723.41499999999996</v>
+      </c>
+      <c r="O31" s="10">
         <f>E31</f>
-        <v>15.198</v>
+        <v>738.56200000000001</v>
       </c>
       <c r="P31" s="10">
-        <v>17.177</v>
+        <v>755.827</v>
       </c>
       <c r="Q31" s="15">
-        <v>18.030999999999999</v>
+        <v>793.55499999999995</v>
       </c>
       <c r="R31" s="10"/>
       <c r="S31" s="10"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10">
-        <v>19.335999999999999</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="E32" s="15">
-        <v>26.244</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="J32" s="10"/>
       <c r="K32" s="10">
         <f>D32</f>
-        <v>19.335999999999999</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10">
-        <v>26.01</v>
-      </c>
-      <c r="O32" s="143">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="O32" s="10">
         <f>E32</f>
-        <v>26.244</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="P32" s="10">
-        <v>29.803999999999998</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="Q32" s="15">
-        <v>31.149000000000001</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="R32" s="10"/>
       <c r="S32" s="10"/>
     </row>
-    <row r="33" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="11">
-        <f>SUM(C28:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="11">
-        <f>SUM(D28:D32)</f>
-        <v>427.50299999999999</v>
-      </c>
-      <c r="E33" s="14">
-        <f>SUM(E28:E32)</f>
-        <v>803.48900000000003</v>
-      </c>
-      <c r="J33" s="11">
-        <f t="shared" ref="J33:O33" si="21">SUM(J28:J32)</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="11">
-        <f t="shared" si="21"/>
-        <v>427.50299999999999</v>
-      </c>
-      <c r="L33" s="11">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="11">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="11">
-        <f t="shared" si="21"/>
-        <v>781.35199999999986</v>
-      </c>
-      <c r="O33" s="144">
-        <f t="shared" si="21"/>
-        <v>803.48900000000003</v>
-      </c>
-      <c r="P33" s="11">
-        <f t="shared" ref="P33:S33" si="22">SUM(P28:P32)</f>
-        <v>826.44200000000001</v>
-      </c>
-      <c r="Q33" s="14">
-        <f t="shared" si="22"/>
-        <v>872.36299999999994</v>
-      </c>
-      <c r="R33" s="11">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="S33" s="11">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10">
+        <v>10.723000000000001</v>
+      </c>
+      <c r="E33" s="15">
+        <v>23.076000000000001</v>
+      </c>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10">
+        <f>D33</f>
+        <v>10.723000000000001</v>
+      </c>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10">
+        <v>17.38</v>
+      </c>
+      <c r="O33" s="10">
+        <f>E33</f>
+        <v>23.076000000000001</v>
+      </c>
+      <c r="P33" s="10">
+        <v>23.241</v>
+      </c>
+      <c r="Q33" s="15">
+        <v>29.225999999999999</v>
+      </c>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>72</v>
+        <v>159</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10">
-        <v>45.837000000000003</v>
+        <v>11.215</v>
       </c>
       <c r="E34" s="15">
-        <v>43.45</v>
+        <v>15.198</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10">
         <f>D34</f>
-        <v>45.837000000000003</v>
+        <v>11.215</v>
       </c>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10">
-        <v>42.73</v>
-      </c>
-      <c r="O34" s="143">
+        <v>14.161</v>
+      </c>
+      <c r="O34" s="10">
         <f>E34</f>
-        <v>43.45</v>
+        <v>15.198</v>
       </c>
       <c r="P34" s="10">
-        <v>42.786000000000001</v>
+        <v>17.177</v>
       </c>
       <c r="Q34" s="15">
-        <v>44.366999999999997</v>
+        <v>18.030999999999999</v>
       </c>
       <c r="R34" s="10"/>
       <c r="S34" s="10"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10">
-        <v>45.695</v>
+        <v>19.335999999999999</v>
       </c>
       <c r="E35" s="15">
-        <v>36.987000000000002</v>
+        <v>26.244</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="10">
         <f>D35</f>
-        <v>45.695</v>
+        <v>19.335999999999999</v>
       </c>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10">
-        <v>39.506</v>
-      </c>
-      <c r="O35" s="143">
+        <v>26.01</v>
+      </c>
+      <c r="O35" s="10">
         <f>E35</f>
-        <v>36.987000000000002</v>
+        <v>26.244</v>
       </c>
       <c r="P35" s="10">
-        <v>34.683999999999997</v>
+        <v>29.803999999999998</v>
       </c>
       <c r="Q35" s="15">
-        <v>32.073</v>
+        <v>31.149000000000001</v>
       </c>
       <c r="R35" s="10"/>
       <c r="S35" s="10"/>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>159</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10">
-        <v>15.983000000000001</v>
-      </c>
-      <c r="E36" s="15">
-        <v>23.177</v>
-      </c>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10">
-        <f>D36</f>
-        <v>15.983000000000001</v>
-      </c>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10">
-        <v>20.687000000000001</v>
-      </c>
-      <c r="O36" s="143">
-        <f>E36</f>
-        <v>23.177</v>
-      </c>
-      <c r="P36" s="10">
-        <v>24.507000000000001</v>
-      </c>
-      <c r="Q36" s="15">
-        <v>26.696000000000002</v>
-      </c>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
+    <row r="36" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="11">
+        <f>SUM(C31:C35)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="11">
+        <f>SUM(D31:D35)</f>
+        <v>427.50299999999999</v>
+      </c>
+      <c r="E36" s="14">
+        <f>SUM(E31:E35)</f>
+        <v>803.48900000000003</v>
+      </c>
+      <c r="J36" s="11">
+        <f t="shared" ref="J36:O36" si="22">SUM(J31:J35)</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="11">
+        <f t="shared" si="22"/>
+        <v>427.50299999999999</v>
+      </c>
+      <c r="L36" s="11">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="11">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="11">
+        <f t="shared" si="22"/>
+        <v>781.35199999999986</v>
+      </c>
+      <c r="O36" s="11">
+        <f t="shared" si="22"/>
+        <v>803.48900000000003</v>
+      </c>
+      <c r="P36" s="11">
+        <f t="shared" ref="P36:S36" si="23">SUM(P31:P35)</f>
+        <v>826.44200000000001</v>
+      </c>
+      <c r="Q36" s="14">
+        <f t="shared" si="23"/>
+        <v>872.36299999999994</v>
+      </c>
+      <c r="R36" s="11">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="S36" s="11">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10">
-        <v>0.68700000000000006</v>
+        <v>45.837000000000003</v>
       </c>
       <c r="E37" s="15">
-        <v>0.68600000000000005</v>
+        <v>43.45</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10">
-        <f>D37</f>
-        <v>0.68700000000000006</v>
+        <f t="shared" ref="K37:K42" si="24">D37</f>
+        <v>45.837000000000003</v>
       </c>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="O37" s="143">
-        <f>E37</f>
-        <v>0.68600000000000005</v>
+        <v>42.73</v>
+      </c>
+      <c r="O37" s="10">
+        <f t="shared" ref="O37:O42" si="25">E37</f>
+        <v>43.45</v>
       </c>
       <c r="P37" s="10">
-        <v>0.65700000000000003</v>
+        <v>42.786000000000001</v>
       </c>
       <c r="Q37" s="15">
-        <v>0.67200000000000004</v>
+        <v>44.366999999999997</v>
       </c>
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
     </row>
-    <row r="38" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10">
-        <v>84.415000000000006</v>
+        <v>45.695</v>
       </c>
       <c r="E38" s="15">
-        <v>173.84399999999999</v>
+        <v>36.987000000000002</v>
       </c>
       <c r="J38" s="10"/>
       <c r="K38" s="10">
-        <f>D38</f>
-        <v>84.415000000000006</v>
+        <f t="shared" si="24"/>
+        <v>45.695</v>
       </c>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10">
-        <v>178.96799999999999</v>
-      </c>
-      <c r="O38" s="143">
-        <f>E38</f>
-        <v>173.84399999999999</v>
+        <v>39.506</v>
+      </c>
+      <c r="O38" s="10">
+        <f t="shared" si="25"/>
+        <v>36.987000000000002</v>
       </c>
       <c r="P38" s="10">
-        <v>168.72</v>
+        <v>34.683999999999997</v>
       </c>
       <c r="Q38" s="15">
-        <v>163.595</v>
+        <v>32.073</v>
       </c>
       <c r="R38" s="10"/>
       <c r="S38" s="10"/>
     </row>
-    <row r="39" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>21</v>
+        <v>159</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10">
-        <v>8.9589999999999996</v>
+        <v>15.983000000000001</v>
       </c>
       <c r="E39" s="15">
-        <v>7.4169999999999998</v>
+        <v>23.177</v>
       </c>
       <c r="J39" s="10"/>
       <c r="K39" s="10">
-        <f>D39</f>
-        <v>8.9589999999999996</v>
+        <f t="shared" si="24"/>
+        <v>15.983000000000001</v>
       </c>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10">
-        <v>7.5330000000000004</v>
-      </c>
-      <c r="O39" s="143">
-        <f>E39</f>
-        <v>7.4169999999999998</v>
+        <v>20.687000000000001</v>
+      </c>
+      <c r="O39" s="10">
+        <f t="shared" si="25"/>
+        <v>23.177</v>
       </c>
       <c r="P39" s="10">
-        <v>10.6</v>
+        <v>24.507000000000001</v>
       </c>
       <c r="Q39" s="15">
-        <v>10.071999999999999</v>
+        <v>26.696000000000002</v>
       </c>
       <c r="R39" s="10"/>
       <c r="S39" s="10"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="11">
-        <f>SUM(C33:C39)</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="11">
-        <f>SUM(D33:D39)</f>
-        <v>629.07899999999984</v>
-      </c>
-      <c r="E40" s="14">
-        <f>SUM(E33:E39)</f>
-        <v>1089.05</v>
-      </c>
-      <c r="J40" s="11">
-        <f t="shared" ref="J40:O40" si="23">SUM(J33:J39)</f>
-        <v>0</v>
-      </c>
-      <c r="K40" s="11">
-        <f t="shared" si="23"/>
-        <v>629.07899999999984</v>
-      </c>
-      <c r="L40" s="11">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M40" s="11">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="N40" s="11">
-        <f t="shared" si="23"/>
-        <v>1071.4239999999998</v>
-      </c>
-      <c r="O40" s="144">
-        <f t="shared" si="23"/>
-        <v>1089.05</v>
-      </c>
-      <c r="P40" s="11">
-        <f t="shared" ref="P40:S40" si="24">SUM(P33:P39)</f>
-        <v>1108.396</v>
-      </c>
-      <c r="Q40" s="14">
+      <c r="B40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="E40" s="15">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10">
         <f t="shared" si="24"/>
-        <v>1149.8379999999997</v>
-      </c>
-      <c r="R40" s="11">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="S40" s="11">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="O40" s="10">
+        <f t="shared" si="25"/>
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="P40" s="10">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="Q40" s="15">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+    </row>
+    <row r="41" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>24</v>
+        <v>161</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10">
-        <v>8.89</v>
+        <v>84.415000000000006</v>
       </c>
       <c r="E41" s="15">
-        <v>13.597</v>
+        <v>173.84399999999999</v>
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="10">
-        <f>D41</f>
-        <v>8.89</v>
+        <f t="shared" si="24"/>
+        <v>84.415000000000006</v>
       </c>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10">
-        <v>9.7379999999999995</v>
-      </c>
-      <c r="O41" s="143">
-        <f>E41</f>
-        <v>13.597</v>
+        <v>178.96799999999999</v>
+      </c>
+      <c r="O41" s="10">
+        <f t="shared" si="25"/>
+        <v>173.84399999999999</v>
       </c>
       <c r="P41" s="10">
-        <v>8.4640000000000004</v>
+        <v>168.72</v>
       </c>
       <c r="Q41" s="15">
-        <v>9.4179999999999993</v>
+        <v>163.595</v>
       </c>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
     </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>162</v>
+        <v>21</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10">
-        <v>36.125999999999998</v>
+        <v>8.9589999999999996</v>
       </c>
       <c r="E42" s="15">
-        <v>62.838000000000001</v>
+        <v>7.4169999999999998</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10">
-        <f>D42</f>
-        <v>36.125999999999998</v>
+        <f t="shared" si="24"/>
+        <v>8.9589999999999996</v>
       </c>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10">
-        <v>62.601999999999997</v>
-      </c>
-      <c r="O42" s="143">
-        <f>E42</f>
-        <v>62.838000000000001</v>
+        <v>7.5330000000000004</v>
+      </c>
+      <c r="O42" s="10">
+        <f t="shared" si="25"/>
+        <v>7.4169999999999998</v>
       </c>
       <c r="P42" s="10">
-        <v>65.134</v>
+        <v>10.6</v>
       </c>
       <c r="Q42" s="15">
-        <v>62.404000000000003</v>
+        <v>10.071999999999999</v>
       </c>
       <c r="R42" s="10"/>
       <c r="S42" s="10"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>163</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10">
-        <v>14.864000000000001</v>
-      </c>
-      <c r="E43" s="15">
-        <v>14.081</v>
-      </c>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10">
-        <f>D43</f>
-        <v>14.864000000000001</v>
-      </c>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10">
-        <v>14.449</v>
-      </c>
-      <c r="O43" s="143">
-        <f>E43</f>
-        <v>14.081</v>
-      </c>
-      <c r="P43" s="10">
-        <v>13.625</v>
-      </c>
-      <c r="Q43" s="15">
-        <v>13.009</v>
-      </c>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
+      <c r="B43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="11">
+        <f>SUM(C36:C42)</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="11">
+        <f>SUM(D36:D42)</f>
+        <v>629.07899999999984</v>
+      </c>
+      <c r="E43" s="14">
+        <f>SUM(E36:E42)</f>
+        <v>1089.05</v>
+      </c>
+      <c r="J43" s="11">
+        <f t="shared" ref="J43:O43" si="26">SUM(J36:J42)</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="11">
+        <f t="shared" si="26"/>
+        <v>629.07899999999984</v>
+      </c>
+      <c r="L43" s="11">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="11">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="11">
+        <f t="shared" si="26"/>
+        <v>1071.4239999999998</v>
+      </c>
+      <c r="O43" s="11">
+        <f t="shared" si="26"/>
+        <v>1089.05</v>
+      </c>
+      <c r="P43" s="11">
+        <f t="shared" ref="P43:S43" si="27">SUM(P36:P42)</f>
+        <v>1108.396</v>
+      </c>
+      <c r="Q43" s="14">
+        <f t="shared" si="27"/>
+        <v>1149.8379999999997</v>
+      </c>
+      <c r="R43" s="11">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="S43" s="11">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>164</v>
+        <v>24</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10">
-        <v>25.109000000000002</v>
+        <v>8.89</v>
       </c>
       <c r="E44" s="15">
-        <v>40.1</v>
+        <v>13.597</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10">
         <f>D44</f>
-        <v>25.109000000000002</v>
+        <v>8.89</v>
       </c>
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
       <c r="N44" s="10">
-        <v>32.866</v>
-      </c>
-      <c r="O44" s="143">
+        <v>9.7379999999999995</v>
+      </c>
+      <c r="O44" s="10">
         <f>E44</f>
-        <v>40.1</v>
+        <v>13.597</v>
       </c>
       <c r="P44" s="10">
-        <v>42.518999999999998</v>
+        <v>8.4640000000000004</v>
       </c>
       <c r="Q44" s="15">
-        <v>46.781999999999996</v>
+        <v>9.4179999999999993</v>
       </c>
       <c r="R44" s="10"/>
       <c r="S44" s="10"/>
     </row>
-    <row r="45" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="11">
-        <f>SUM(C41:C44)</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="11">
-        <f>SUM(D41:D44)</f>
-        <v>84.989000000000004</v>
-      </c>
-      <c r="E45" s="14">
-        <f>SUM(E41:E44)</f>
-        <v>130.61600000000001</v>
-      </c>
-      <c r="J45" s="11">
-        <f t="shared" ref="J45:O45" si="25">SUM(J41:J44)</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="11">
-        <f t="shared" si="25"/>
-        <v>84.989000000000004</v>
-      </c>
-      <c r="L45" s="11">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="11">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="N45" s="11">
-        <f t="shared" si="25"/>
-        <v>119.655</v>
-      </c>
-      <c r="O45" s="144">
-        <f t="shared" si="25"/>
-        <v>130.61600000000001</v>
-      </c>
-      <c r="P45" s="11">
-        <f t="shared" ref="P45:S45" si="26">SUM(P41:P44)</f>
-        <v>129.74199999999999</v>
-      </c>
-      <c r="Q45" s="14">
-        <f t="shared" si="26"/>
-        <v>131.613</v>
-      </c>
-      <c r="R45" s="11">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="S45" s="11">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10">
+        <v>36.125999999999998</v>
+      </c>
+      <c r="E45" s="15">
+        <v>62.838000000000001</v>
+      </c>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10">
+        <f>D45</f>
+        <v>36.125999999999998</v>
+      </c>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10">
+        <v>62.601999999999997</v>
+      </c>
+      <c r="O45" s="10">
+        <f>E45</f>
+        <v>62.838000000000001</v>
+      </c>
+      <c r="P45" s="10">
+        <v>65.134</v>
+      </c>
+      <c r="Q45" s="15">
+        <v>62.404000000000003</v>
+      </c>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -14500,198 +14477,320 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10">
-        <v>47.543999999999997</v>
+        <v>14.864000000000001</v>
       </c>
       <c r="E46" s="15">
-        <v>37.497999999999998</v>
+        <v>14.081</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10">
         <f>D46</f>
-        <v>47.543999999999997</v>
+        <v>14.864000000000001</v>
       </c>
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
       <c r="N46" s="10">
-        <v>40.015999999999998</v>
-      </c>
-      <c r="O46" s="143">
+        <v>14.449</v>
+      </c>
+      <c r="O46" s="10">
         <f>E46</f>
-        <v>37.497999999999998</v>
+        <v>14.081</v>
       </c>
       <c r="P46" s="10">
-        <v>34.759</v>
+        <v>13.625</v>
       </c>
       <c r="Q46" s="15">
-        <v>32.069000000000003</v>
+        <v>13.009</v>
       </c>
       <c r="R46" s="10"/>
       <c r="S46" s="10"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>20</v>
+        <v>164</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10">
-        <v>0.876</v>
+        <v>25.109000000000002</v>
       </c>
       <c r="E47" s="15">
-        <v>6.1589999999999998</v>
+        <v>40.1</v>
       </c>
       <c r="J47" s="10"/>
       <c r="K47" s="10">
         <f>D47</f>
-        <v>0.876</v>
+        <v>25.109000000000002</v>
       </c>
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
       <c r="N47" s="10">
-        <v>6.4089999999999998</v>
-      </c>
-      <c r="O47" s="143">
+        <v>32.866</v>
+      </c>
+      <c r="O47" s="10">
         <f>E47</f>
-        <v>6.1589999999999998</v>
+        <v>40.1</v>
       </c>
       <c r="P47" s="10">
-        <v>6.4429999999999996</v>
+        <v>42.518999999999998</v>
       </c>
       <c r="Q47" s="15">
-        <v>6.6559999999999997</v>
+        <v>46.781999999999996</v>
       </c>
       <c r="R47" s="10"/>
       <c r="S47" s="10"/>
     </row>
-    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C48" s="11">
-        <f>SUM(C45:C47)</f>
+        <f>SUM(C44:C47)</f>
         <v>0</v>
       </c>
       <c r="D48" s="11">
-        <f>SUM(D45:D47)</f>
-        <v>133.40900000000002</v>
+        <f>SUM(D44:D47)</f>
+        <v>84.989000000000004</v>
       </c>
       <c r="E48" s="14">
-        <f>SUM(E45:E47)</f>
-        <v>174.273</v>
+        <f>SUM(E44:E47)</f>
+        <v>130.61600000000001</v>
       </c>
       <c r="J48" s="11">
-        <f t="shared" ref="J48:O48" si="27">SUM(J45:J47)</f>
+        <f t="shared" ref="J48:O48" si="28">SUM(J44:J47)</f>
         <v>0</v>
       </c>
       <c r="K48" s="11">
-        <f t="shared" si="27"/>
-        <v>133.40900000000002</v>
+        <f t="shared" si="28"/>
+        <v>84.989000000000004</v>
       </c>
       <c r="L48" s="11">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="11">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="N48" s="11">
-        <f t="shared" si="27"/>
-        <v>166.07999999999998</v>
-      </c>
-      <c r="O48" s="144">
-        <f t="shared" si="27"/>
-        <v>174.273</v>
-      </c>
-      <c r="P48" s="11">
-        <f t="shared" ref="P48:S48" si="28">SUM(P45:P47)</f>
-        <v>170.94399999999999</v>
-      </c>
-      <c r="Q48" s="14">
-        <f t="shared" si="28"/>
-        <v>170.33800000000002</v>
-      </c>
-      <c r="R48" s="11">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="S48" s="11">
+      <c r="M48" s="11">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
+      <c r="N48" s="11">
+        <f t="shared" si="28"/>
+        <v>119.655</v>
+      </c>
+      <c r="O48" s="11">
+        <f t="shared" si="28"/>
+        <v>130.61600000000001</v>
+      </c>
+      <c r="P48" s="11">
+        <f t="shared" ref="P48:S48" si="29">SUM(P44:P47)</f>
+        <v>129.74199999999999</v>
+      </c>
+      <c r="Q48" s="14">
+        <f t="shared" si="29"/>
+        <v>131.613</v>
+      </c>
+      <c r="R48" s="11">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="S48" s="11">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10">
-        <f>D40-D48</f>
-        <v>495.66999999999985</v>
+        <v>47.543999999999997</v>
       </c>
       <c r="E49" s="15">
-        <f>E40-E48</f>
-        <v>914.77699999999993</v>
-      </c>
-      <c r="J49" s="10">
-        <f>J40-J48</f>
+        <v>37.497999999999998</v>
+      </c>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10">
+        <f>D49</f>
+        <v>47.543999999999997</v>
+      </c>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10">
+        <v>40.015999999999998</v>
+      </c>
+      <c r="O49" s="10">
+        <f>E49</f>
+        <v>37.497999999999998</v>
+      </c>
+      <c r="P49" s="10">
+        <v>34.759</v>
+      </c>
+      <c r="Q49" s="15">
+        <v>32.069000000000003</v>
+      </c>
+      <c r="R49" s="10"/>
+      <c r="S49" s="10"/>
+    </row>
+    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10">
+        <v>0.876</v>
+      </c>
+      <c r="E50" s="15">
+        <v>6.1589999999999998</v>
+      </c>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10">
+        <f>D50</f>
+        <v>0.876</v>
+      </c>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10">
+        <v>6.4089999999999998</v>
+      </c>
+      <c r="O50" s="10">
+        <f>E50</f>
+        <v>6.1589999999999998</v>
+      </c>
+      <c r="P50" s="10">
+        <v>6.4429999999999996</v>
+      </c>
+      <c r="Q50" s="15">
+        <v>6.6559999999999997</v>
+      </c>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="11">
+        <f>SUM(C48:C50)</f>
         <v>0</v>
       </c>
-      <c r="K49" s="10">
-        <f>K40-K48</f>
-        <v>495.66999999999985</v>
-      </c>
-      <c r="L49" s="10">
-        <f t="shared" ref="L49:O49" si="29">L40-L48</f>
+      <c r="D51" s="11">
+        <f>SUM(D48:D50)</f>
+        <v>133.40900000000002</v>
+      </c>
+      <c r="E51" s="14">
+        <f>SUM(E48:E50)</f>
+        <v>174.273</v>
+      </c>
+      <c r="J51" s="11">
+        <f t="shared" ref="J51:O51" si="30">SUM(J48:J50)</f>
         <v>0</v>
       </c>
-      <c r="M49" s="10">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N49" s="10">
-        <f t="shared" si="29"/>
-        <v>905.34399999999982</v>
-      </c>
-      <c r="O49" s="143">
-        <f t="shared" si="29"/>
-        <v>914.77699999999993</v>
-      </c>
-      <c r="P49" s="10">
-        <f t="shared" ref="P49:S49" si="30">P40-P48</f>
-        <v>937.452</v>
-      </c>
-      <c r="Q49" s="15">
+      <c r="K51" s="11">
         <f t="shared" si="30"/>
-        <v>979.49999999999977</v>
-      </c>
-      <c r="R49" s="10">
+        <v>133.40900000000002</v>
+      </c>
+      <c r="L51" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="S49" s="10">
+      <c r="M51" s="11">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
+      <c r="N51" s="11">
+        <f t="shared" si="30"/>
+        <v>166.07999999999998</v>
+      </c>
+      <c r="O51" s="11">
+        <f t="shared" si="30"/>
+        <v>174.273</v>
+      </c>
+      <c r="P51" s="11">
+        <f t="shared" ref="P51:S51" si="31">SUM(P48:P50)</f>
+        <v>170.94399999999999</v>
+      </c>
+      <c r="Q51" s="14">
+        <f t="shared" si="31"/>
+        <v>170.33800000000002</v>
+      </c>
+      <c r="R51" s="11">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="S51" s="11">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10">
+        <f>D43-D51</f>
+        <v>495.66999999999985</v>
+      </c>
+      <c r="E52" s="15">
+        <f>E43-E51</f>
+        <v>914.77699999999993</v>
+      </c>
+      <c r="J52" s="10">
+        <f>J43-J51</f>
+        <v>0</v>
+      </c>
+      <c r="K52" s="10">
+        <f>K43-K51</f>
+        <v>495.66999999999985</v>
+      </c>
+      <c r="L52" s="10">
+        <f t="shared" ref="L52:O52" si="32">L43-L51</f>
+        <v>0</v>
+      </c>
+      <c r="M52" s="10">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="N52" s="10">
+        <f t="shared" si="32"/>
+        <v>905.34399999999982</v>
+      </c>
+      <c r="O52" s="10">
+        <f t="shared" si="32"/>
+        <v>914.77699999999993</v>
+      </c>
+      <c r="P52" s="10">
+        <f t="shared" ref="P52:S52" si="33">P43-P51</f>
+        <v>937.452</v>
+      </c>
+      <c r="Q52" s="15">
+        <f t="shared" si="33"/>
+        <v>979.49999999999977</v>
+      </c>
+      <c r="R52" s="10">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="S52" s="10">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="52"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="53"/>
-      <c r="O51" s="148"/>
-      <c r="Q51" s="16"/>
-    </row>
-    <row r="69" spans="5:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E69" s="41"/>
-      <c r="O69" s="149"/>
-      <c r="Q69" s="41"/>
-    </row>
-    <row r="70" spans="5:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E70" s="16"/>
-      <c r="O70" s="148"/>
-      <c r="Q70" s="16"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="53"/>
+      <c r="Q54" s="16"/>
+    </row>
+    <row r="72" spans="5:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E72" s="41"/>
+      <c r="Q72" s="41"/>
+    </row>
+    <row r="73" spans="5:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="16"/>
+      <c r="Q73" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -23295,14 +23394,14 @@
       <c r="D1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="132" t="s">
+      <c r="H1" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="134"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="137"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12">
@@ -23805,10 +23904,10 @@
         <f t="shared" si="0"/>
         <v>-4.9391717325228957E-3</v>
       </c>
-      <c r="H17" s="135" t="s">
+      <c r="H17" s="138" t="s">
         <v>127</v>
       </c>
-      <c r="I17" s="136"/>
+      <c r="I17" s="139"/>
       <c r="M17" s="83"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -23822,8 +23921,8 @@
         <f t="shared" si="0"/>
         <v>-5.2555829641618756E-2</v>
       </c>
-      <c r="H18" s="137"/>
-      <c r="I18" s="138"/>
+      <c r="H18" s="140"/>
+      <c r="I18" s="141"/>
       <c r="M18" s="83"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -24292,14 +24391,14 @@
       <c r="M42" s="96"/>
     </row>
     <row r="43" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H43" s="139" t="s">
+      <c r="H43" s="142" t="s">
         <v>121</v>
       </c>
-      <c r="I43" s="140"/>
-      <c r="J43" s="140"/>
-      <c r="K43" s="140"/>
-      <c r="L43" s="140"/>
-      <c r="M43" s="141"/>
+      <c r="I43" s="143"/>
+      <c r="J43" s="143"/>
+      <c r="K43" s="143"/>
+      <c r="L43" s="143"/>
+      <c r="M43" s="144"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H44" s="97">

</xml_diff>